<commit_message>
Update slides and rubric
</commit_message>
<xml_diff>
--- a/Module 4/Week 10/White Paper Rubric.xlsx
+++ b/Module 4/Week 10/White Paper Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdmeu\Documents\Teaching\GEOG 463-563\Sp2025\Module 4\Week 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97CD63B-5394-45CF-B31E-E20BD2E38D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFFD15E-F2E7-4A51-94B6-1656822AF8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53880" yWindow="-6615" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6675" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -221,6 +221,72 @@
     <t>Recommendation is actionable and effectively addresses the stated problem.</t>
   </si>
   <si>
+    <t>1 page maximum</t>
+  </si>
+  <si>
+    <t>a. Summary of problem</t>
+  </si>
+  <si>
+    <t>b. Summary of solutions</t>
+  </si>
+  <si>
+    <t>c. Summary of recommendations</t>
+  </si>
+  <si>
+    <t>The consequences of maintaining the status quo (i.e., doing nothing) are weighed for each stakeholder group.</t>
+  </si>
+  <si>
+    <t>The intended audience for the white paper and affected stakeholders are described.</t>
+  </si>
+  <si>
+    <t>The case for addressing the problem is restated.</t>
+  </si>
+  <si>
+    <t>The possible solutions and their impacts on stakeholders are summarized.</t>
+  </si>
+  <si>
+    <t>The recommendations made to address the problem are summarized with a look ahead toward follow-up efforts.</t>
+  </si>
+  <si>
+    <t>The most important points from the background section are described concisely.</t>
+  </si>
+  <si>
+    <t>The most important points from the problem description section are described concisely.</t>
+  </si>
+  <si>
+    <t>The most important points from the solution description section are described concisely.</t>
+  </si>
+  <si>
+    <t>The most important points from the recommendations section are described concisely.</t>
+  </si>
+  <si>
+    <t>The values of each stakeholder group are defined, and the impacts are related to these values.</t>
+  </si>
+  <si>
+    <t>a. Acceptable solution criteria</t>
+  </si>
+  <si>
+    <t>b. First solution</t>
+  </si>
+  <si>
+    <t>c. Second solution</t>
+  </si>
+  <si>
+    <t>d. Reasoning</t>
+  </si>
+  <si>
+    <t>All criteria that must be fulfilled by the proposed solutions are described. Criteria must be both necessary (i.e., essential to solve the problem) and sufficient (i.e., all-encompassing for solving the problem).</t>
+  </si>
+  <si>
+    <t>c. Feasibility and efficacy</t>
+  </si>
+  <si>
+    <t>At least 30 appropriate sources are cited.</t>
+  </si>
+  <si>
+    <t>Correct and consistent citation style is used.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Recommendations are made from the available solutions, and intended impacts on stakeholders are described. </t>
     </r>
@@ -241,74 +307,8 @@
         <rFont val="Aptos"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> is provided to support this recommendation. Add a timeline or workplan if relevant.</t>
+      <t xml:space="preserve"> is provided to support this recommendation. A timeline or workplan is included if relevant.</t>
     </r>
-  </si>
-  <si>
-    <t>1 page maximum</t>
-  </si>
-  <si>
-    <t>a. Summary of problem</t>
-  </si>
-  <si>
-    <t>b. Summary of solutions</t>
-  </si>
-  <si>
-    <t>c. Summary of recommendations</t>
-  </si>
-  <si>
-    <t>The consequences of maintaining the status quo (i.e., doing nothing) are weighed for each stakeholder group.</t>
-  </si>
-  <si>
-    <t>The intended audience for the white paper and affected stakeholders are described.</t>
-  </si>
-  <si>
-    <t>The case for addressing the problem is restated.</t>
-  </si>
-  <si>
-    <t>The possible solutions and their impacts on stakeholders are summarized.</t>
-  </si>
-  <si>
-    <t>The recommendations made to address the problem are summarized with a look ahead toward follow-up efforts.</t>
-  </si>
-  <si>
-    <t>The most important points from the background section are described concisely.</t>
-  </si>
-  <si>
-    <t>The most important points from the problem description section are described concisely.</t>
-  </si>
-  <si>
-    <t>The most important points from the solution description section are described concisely.</t>
-  </si>
-  <si>
-    <t>The most important points from the recommendations section are described concisely.</t>
-  </si>
-  <si>
-    <t>The values of each stakeholder group are defined, and the impacts are related to these values.</t>
-  </si>
-  <si>
-    <t>a. Acceptable solution criteria</t>
-  </si>
-  <si>
-    <t>b. First solution</t>
-  </si>
-  <si>
-    <t>c. Second solution</t>
-  </si>
-  <si>
-    <t>d. Reasoning</t>
-  </si>
-  <si>
-    <t>All criteria that must be fulfilled by the proposed solutions are described. Criteria must be both necessary (i.e., essential to solve the problem) and sufficient (i.e., all-encompassing for solving the problem).</t>
-  </si>
-  <si>
-    <t>c. Feasibility and efficacy</t>
-  </si>
-  <si>
-    <t>At least 30 appropriate sources are cited.</t>
-  </si>
-  <si>
-    <t>Correct and consistent citation style is used.</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -388,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -397,44 +397,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,19 +701,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.21875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="51.77734375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="28.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="51.77734375" style="4" customWidth="1"/>
     <col min="6" max="16" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -764,12 +748,12 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="11">
+        <v>40</v>
+      </c>
+      <c r="C2" s="10">
         <v>2</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <f>SUM(D3:D4)</f>
         <v>0</v>
       </c>
@@ -782,10 +766,10 @@
       <c r="B3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>1</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -795,10 +779,10 @@
       <c r="B4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -806,12 +790,12 @@
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="11">
+        <v>40</v>
+      </c>
+      <c r="C5" s="10">
         <v>15</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -819,12 +803,12 @@
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="12">
+        <v>49</v>
+      </c>
+      <c r="C6" s="11">
         <v>3</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -832,12 +816,12 @@
         <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="12">
+        <v>50</v>
+      </c>
+      <c r="C7" s="11">
         <v>4</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -845,12 +829,12 @@
         <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="12">
+        <v>51</v>
+      </c>
+      <c r="C8" s="11">
         <v>4</v>
       </c>
-      <c r="D8" s="12"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -858,12 +842,12 @@
         <v>14</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="12">
+        <v>52</v>
+      </c>
+      <c r="C9" s="11">
         <v>4</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -871,10 +855,10 @@
         <v>25</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>15</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -884,10 +868,10 @@
       <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>6</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -897,10 +881,10 @@
       <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>6</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -908,12 +892,12 @@
         <v>30</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="12">
+        <v>45</v>
+      </c>
+      <c r="C13" s="11">
         <v>3</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -921,10 +905,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>17</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
@@ -934,10 +918,10 @@
       <c r="B15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>9</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -945,223 +929,212 @@
         <v>24</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="12">
+        <v>53</v>
+      </c>
+      <c r="C16" s="11">
         <v>4</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="12">
+        <v>44</v>
+      </c>
+      <c r="C17" s="11">
         <v>4</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>18</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:16" s="20" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="11">
+        <v>3</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="18">
-        <v>3</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-    </row>
-    <row r="20" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>6</v>
       </c>
-      <c r="D20" s="12"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>6</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <v>3</v>
       </c>
-      <c r="D22" s="12"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="11">
+      <c r="C23" s="10">
         <v>16</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="12">
+        <v>62</v>
+      </c>
+      <c r="C24" s="11">
         <v>10</v>
       </c>
-      <c r="D24" s="12"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <v>3</v>
       </c>
-      <c r="D25" s="12"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <v>3</v>
       </c>
-      <c r="D26" s="12"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="11">
+      <c r="C27" s="10">
         <v>9</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="11">
+        <v>3</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C29" s="11">
         <v>3</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="D29" s="11"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C30" s="11">
         <v>3</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="12">
-        <v>3</v>
-      </c>
-      <c r="D30" s="12"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <v>8</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="12">
+        <v>60</v>
+      </c>
+      <c r="C32" s="11">
         <v>4</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1169,49 +1142,28 @@
         <v>18</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="13">
+        <v>61</v>
+      </c>
+      <c r="C33" s="12">
         <v>4</v>
       </c>
-      <c r="D33" s="13"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="7"/>
-      <c r="C34" s="12">
+      <c r="C34" s="11">
         <f>C2+C5+C10+C14+C18+C23+C27+C31</f>
         <v>100</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="11">
         <f>D2+D5+D10+D14+D18+D23+D27+D31</f>
         <v>0</v>
       </c>
       <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>